<commit_message>
v.1.2.1; rerun distractor analysis for simulated example in fixture/ex3 because of changes when using use_wle = TRUE
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/ex3/tables/distractors_items.xlsx
+++ b/tests/testthat/fixtures/ex3/tables/distractors_items.xlsx
@@ -455,7 +455,7 @@
         <v>122</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.227</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="3">
@@ -466,7 +466,7 @@
         <v>130</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.252</v>
+        <v>-0.266</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +477,7 @@
         <v>1612</v>
       </c>
       <c r="C4" t="n">
-        <v>0.442</v>
+        <v>0.467</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>121</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.233</v>
+        <v>-0.246</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +524,7 @@
         <v>109</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.23</v>
+        <v>-0.243</v>
       </c>
     </row>
     <row r="3">
@@ -535,7 +535,7 @@
         <v>95</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.199</v>
+        <v>-0.211</v>
       </c>
     </row>
     <row r="4">
@@ -546,7 +546,7 @@
         <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.265</v>
+        <v>-0.277</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         <v>318</v>
       </c>
       <c r="C5" t="n">
-        <v>0.513</v>
+        <v>0.54</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +593,7 @@
         <v>116</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.227</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="3">
@@ -604,7 +604,7 @@
         <v>80</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.166</v>
+        <v>-0.177</v>
       </c>
     </row>
     <row r="4">
@@ -615,7 +615,7 @@
         <v>270</v>
       </c>
       <c r="C4" t="n">
-        <v>0.491</v>
+        <v>0.518</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +626,7 @@
         <v>101</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.25</v>
+        <v>-0.262</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +662,7 @@
         <v>206</v>
       </c>
       <c r="C2" t="n">
-        <v>0.485</v>
+        <v>0.511</v>
       </c>
     </row>
     <row r="3">
@@ -673,7 +673,7 @@
         <v>98</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.186</v>
+        <v>-0.198</v>
       </c>
     </row>
     <row r="4">
@@ -684,7 +684,7 @@
         <v>93</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.193</v>
+        <v>-0.204</v>
       </c>
     </row>
     <row r="5">
@@ -695,7 +695,7 @@
         <v>88</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.231</v>
+        <v>-0.241</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +731,7 @@
         <v>122</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.166</v>
+        <v>-0.177</v>
       </c>
     </row>
     <row r="3">
@@ -742,7 +742,7 @@
         <v>132</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.196</v>
+        <v>-0.208</v>
       </c>
     </row>
     <row r="4">
@@ -753,7 +753,7 @@
         <v>266</v>
       </c>
       <c r="C4" t="n">
-        <v>0.508</v>
+        <v>0.537</v>
       </c>
     </row>
     <row r="5">
@@ -764,7 +764,7 @@
         <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.256</v>
+        <v>-0.268</v>
       </c>
     </row>
   </sheetData>
@@ -800,7 +800,7 @@
         <v>139</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.174</v>
+        <v>-0.185</v>
       </c>
     </row>
     <row r="3">
@@ -811,7 +811,7 @@
         <v>138</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.171</v>
+        <v>-0.183</v>
       </c>
     </row>
     <row r="4">
@@ -822,7 +822,7 @@
         <v>147</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.232</v>
+        <v>-0.243</v>
       </c>
     </row>
     <row r="5">
@@ -833,7 +833,7 @@
         <v>254</v>
       </c>
       <c r="C5" t="n">
-        <v>0.484</v>
+        <v>0.514</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +869,7 @@
         <v>159</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.124</v>
+        <v>-0.133</v>
       </c>
     </row>
     <row r="3">
@@ -880,7 +880,7 @@
         <v>186</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.186</v>
+        <v>-0.196</v>
       </c>
     </row>
     <row r="4">
@@ -891,7 +891,7 @@
         <v>152</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.241</v>
+        <v>-0.248</v>
       </c>
     </row>
     <row r="5">
@@ -902,7 +902,7 @@
         <v>179</v>
       </c>
       <c r="C5" t="n">
-        <v>0.536</v>
+        <v>0.56</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +938,7 @@
         <v>156</v>
       </c>
       <c r="C2" t="n">
-        <v>0.496</v>
+        <v>0.521</v>
       </c>
     </row>
     <row r="3">
@@ -949,7 +949,7 @@
         <v>167</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.163</v>
+        <v>-0.171</v>
       </c>
     </row>
     <row r="4">
@@ -960,7 +960,7 @@
         <v>179</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.164</v>
+        <v>-0.172</v>
       </c>
     </row>
     <row r="5">
@@ -971,7 +971,7 @@
         <v>174</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.151</v>
+        <v>-0.159</v>
       </c>
     </row>
   </sheetData>
@@ -1007,7 +1007,7 @@
         <v>337</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.298</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="3">
@@ -1018,7 +1018,7 @@
         <v>926</v>
       </c>
       <c r="C3" t="n">
-        <v>0.52</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="4">
@@ -1029,7 +1029,7 @@
         <v>299</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.186</v>
+        <v>-0.199</v>
       </c>
     </row>
     <row r="5">
@@ -1040,7 +1040,7 @@
         <v>300</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.209</v>
+        <v>-0.222</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1076,7 @@
         <v>357</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.161</v>
+        <v>-0.167</v>
       </c>
     </row>
     <row r="3">
@@ -1087,7 +1087,7 @@
         <v>390</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.115</v>
+        <v>-0.122</v>
       </c>
     </row>
     <row r="4">
@@ -1098,7 +1098,7 @@
         <v>376</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.085</v>
+        <v>-0.092</v>
       </c>
     </row>
     <row r="5">
@@ -1109,7 +1109,7 @@
         <v>256</v>
       </c>
       <c r="C5" t="n">
-        <v>0.411</v>
+        <v>0.435</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1145,7 @@
         <v>46</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.237</v>
+        <v>-0.251</v>
       </c>
     </row>
     <row r="3">
@@ -1156,7 +1156,7 @@
         <v>499</v>
       </c>
       <c r="C3" t="n">
-        <v>0.428</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="4">
@@ -1167,7 +1167,7 @@
         <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.238</v>
+        <v>-0.253</v>
       </c>
     </row>
     <row r="5">
@@ -1178,7 +1178,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.203</v>
+        <v>-0.221</v>
       </c>
     </row>
   </sheetData>
@@ -1214,7 +1214,7 @@
         <v>475</v>
       </c>
       <c r="C2" t="n">
-        <v>0.419</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="3">
@@ -1225,7 +1225,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.192</v>
+        <v>-0.207</v>
       </c>
     </row>
     <row r="4">
@@ -1236,7 +1236,7 @@
         <v>60</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.24</v>
+        <v>-0.256</v>
       </c>
     </row>
     <row r="5">
@@ -1247,7 +1247,7 @@
         <v>65</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.216</v>
+        <v>-0.233</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1283,7 @@
         <v>420</v>
       </c>
       <c r="C2" t="n">
-        <v>0.501</v>
+        <v>0.531</v>
       </c>
     </row>
     <row r="3">
@@ -1294,7 +1294,7 @@
         <v>84</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.302</v>
+        <v>-0.318</v>
       </c>
     </row>
     <row r="4">
@@ -1305,7 +1305,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.225</v>
+        <v>-0.239</v>
       </c>
     </row>
     <row r="5">
@@ -1316,7 +1316,7 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.214</v>
+        <v>-0.23</v>
       </c>
     </row>
   </sheetData>
@@ -1352,7 +1352,7 @@
         <v>90</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.219</v>
+        <v>-0.236</v>
       </c>
     </row>
     <row r="3">
@@ -1363,7 +1363,7 @@
         <v>404</v>
       </c>
       <c r="C3" t="n">
-        <v>0.478</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="4">
@@ -1374,7 +1374,7 @@
         <v>85</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.245</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="5">
@@ -1385,7 +1385,7 @@
         <v>69</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.238</v>
+        <v>-0.252</v>
       </c>
     </row>
   </sheetData>
@@ -1421,7 +1421,7 @@
         <v>431</v>
       </c>
       <c r="C2" t="n">
-        <v>0.51</v>
+        <v>0.537</v>
       </c>
     </row>
     <row r="3">
@@ -1432,7 +1432,7 @@
         <v>81</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.266</v>
+        <v>-0.279</v>
       </c>
     </row>
     <row r="4">
@@ -1443,7 +1443,7 @@
         <v>79</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.238</v>
+        <v>-0.251</v>
       </c>
     </row>
     <row r="5">
@@ -1454,7 +1454,7 @@
         <v>85</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.249</v>
+        <v>-0.262</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1490,7 @@
         <v>90</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.236</v>
+        <v>-0.248</v>
       </c>
     </row>
     <row r="3">
@@ -1501,7 +1501,7 @@
         <v>113</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.254</v>
+        <v>-0.268</v>
       </c>
     </row>
     <row r="4">
@@ -1512,7 +1512,7 @@
         <v>356</v>
       </c>
       <c r="C4" t="n">
-        <v>0.516</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="5">
@@ -1523,7 +1523,7 @@
         <v>84</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.232</v>
+        <v>-0.244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>